<commit_message>
18-12-25-01 Main Sheet Update
</commit_message>
<xml_diff>
--- a/Sheets/AWS-Zero-to-Hero-Sheet.xlsx
+++ b/Sheets/AWS-Zero-to-Hero-Sheet.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>AWS Official Documentations
 https://docs.aws.amazon.com/</t>
@@ -399,6 +399,18 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">VPC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -406,27 +418,17 @@
         <rFont val="Times New Roman"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">VPC </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">Secured Private Network over the Cloud
-</t>
+Public-Private Architecture in VPC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Must to Prepare for</t>
     </r>
   </si>
   <si>
@@ -512,12 +514,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">Rule Number of rules determines the priority of rules.
 </t>
     </r>
@@ -579,6 +575,135 @@
       </rPr>
       <t xml:space="preserve"> using these rules.</t>
     </r>
+  </si>
+  <si>
+    <t>Route53</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It is a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">DNS Service </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> AWS
+Domain Registration: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>We can purchase Domain in AWS</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+Hosted Zones: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Contains DNS Records
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Route53 Health Checks </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">of Web Servers
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Traffic Flow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Resolver </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>-</t>
+    </r>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/documentation-overview/route53/</t>
   </si>
 </sst>
 </file>
@@ -1777,9 +1902,9 @@
   <dimension ref="A1:XCV1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -1940,7 +2065,7 @@
       <c r="G8" s="27"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" ht="96.6" spans="1:7">
+    <row r="9" ht="111" customHeight="1" spans="1:7">
       <c r="A9" s="11">
         <v>3</v>
       </c>
@@ -1971,7 +2096,7 @@
       <c r="G10" s="27"/>
       <c r="H10" s="28"/>
     </row>
-    <row r="11" ht="41.4" spans="1:7">
+    <row r="11" ht="78" customHeight="1" spans="1:7">
       <c r="A11" s="11">
         <v>4</v>
       </c>
@@ -2052,23 +2177,36 @@
       </c>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
+    <row r="16" ht="99" customHeight="1" spans="1:7">
+      <c r="A16" s="11">
+        <v>6</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>29</v>
+      </c>
       <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
+      <c r="D16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="14">
+        <v>46009</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="11"/>
@@ -4203,6 +4341,7 @@
     <hyperlink ref="G9" r:id="rId6" display="https://docs.aws.amazon.com/global-infrastructure/latest/regions/aws-regions-availability-zones.html"/>
     <hyperlink ref="G11" r:id="rId7" display="https://docs.aws.amazon.com/vpc/latest/userguide/what-is-amazon-vpc.html" tooltip="https://docs.aws.amazon.com/vpc/latest/userguide/what-is-amazon-vpc.html"/>
     <hyperlink ref="G13" r:id="rId8" display="https://www.geeksforgeeks.org/computer-networks/difference-between-security-group-and-network-acl-in-aws/"/>
+    <hyperlink ref="G16" r:id="rId9" display="https://aws.amazon.com/documentation-overview/route53/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
19-12-25-01 Main Sheet Update
</commit_message>
<xml_diff>
--- a/Sheets/AWS-Zero-to-Hero-Sheet.xlsx
+++ b/Sheets/AWS-Zero-to-Hero-Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>AWS Official Documentations
 https://docs.aws.amazon.com/</t>
@@ -399,6 +399,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">VPC </t>
     </r>
     <r>
@@ -514,6 +521,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Rule Number of rules determines the priority of rules.
 </t>
     </r>
@@ -581,6 +594,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">It is a </t>
     </r>
     <r>
@@ -704,6 +723,81 @@
   </si>
   <si>
     <t>https://aws.amazon.com/documentation-overview/route53/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - Creating a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>VPC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> which can be used for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Servers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Production Enviroment</t>
+    </r>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -1483,7 +1577,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1571,9 +1665,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1901,19 +1992,19 @@
   <sheetPr/>
   <dimension ref="A1:XCV1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="8.77777777777778" style="3" customWidth="1"/>
     <col min="2" max="2" width="35.5092592592593" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.037037037037" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.462962962963" style="3" customWidth="1"/>
     <col min="4" max="4" width="21.4444444444444" style="3" customWidth="1"/>
-    <col min="5" max="5" width="34.5555555555556" style="3" customWidth="1"/>
+    <col min="5" max="5" width="40.1481481481481" style="3" customWidth="1"/>
     <col min="6" max="6" width="14.8888888888889" style="3" customWidth="1"/>
     <col min="7" max="7" width="38.1203703703704" style="4" customWidth="1"/>
     <col min="8" max="8" width="8.88888888888889" style="5"/>
@@ -2144,7 +2235,7 @@
       <c r="F13" s="14">
         <v>46007</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="29" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2208,13 +2299,21 @@
       <c r="G17" s="27"/>
       <c r="H17" s="28"/>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
+    <row r="18" ht="51" customHeight="1" spans="1:7">
+      <c r="A18" s="11">
+        <v>7</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="D18" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="F18" s="14">
+        <v>46010</v>
+      </c>
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7">

</xml_diff>